<commit_message>
add updated NG data from EIA
</commit_message>
<xml_diff>
--- a/data/NG_PRI_SUM_DCU_NUS_A.xlsx
+++ b/data/NG_PRI_SUM_DCU_NUS_A.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FF448C9-ED86-214A-854C-7220DBE75392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1"/>
+    <workbookView xWindow="4660" yWindow="460" windowWidth="16140" windowHeight="10000"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="1" r:id="rId1"/>
@@ -12,6 +13,14 @@
   </sheets>
   <calcPr calcId="80000" iterateDelta="9.9999999999994451E-4"/>
   <fileRecoveryPr autoRecover="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,13 +66,13 @@
     <t>Release Date:</t>
   </si>
   <si>
-    <t>8/31/2018</t>
+    <t>7/31/2020</t>
   </si>
   <si>
     <t>Next Release Date:</t>
   </si>
   <si>
-    <t>9/28/2018</t>
+    <t>8/31/2020</t>
   </si>
   <si>
     <t>Excel File Name:</t>
@@ -93,7 +102,7 @@
     <t>(202) 586-8800</t>
   </si>
   <si>
-    <t>8/30/2018 3:08:20 PM</t>
+    <t>7/29/2020 8:35:45 PM</t>
   </si>
   <si>
     <t>Data 1: U.S. Natural Gas Prices</t>
@@ -232,22 +241,26 @@
       <sz val="14"/>
       <color indexed="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -258,21 +271,25 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -280,6 +297,7 @@
       <sz val="12"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -287,22 +305,26 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="63"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -713,7 +735,7 @@
   </sheetPr>
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -787,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="17">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>11</v>
@@ -855,7 +877,7 @@
     <hyperlink ref="B7" location="'Data 1'!A1" display="Data 1"/>
     <hyperlink ref="C13" r:id="rId1"/>
     <hyperlink ref="C14" r:id="rId2" display="http://www.eia.gov/"/>
-    <hyperlink ref="C15" r:id="rId3" display="mailto:infoctr@eia.gov_x0003_"/>
+    <hyperlink ref="C15" r:id="rId3" display="mailto:infoctr@eia.gov_x0003__x0003_MacroGetTooltip"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -868,9 +890,9 @@
   <sheetPr>
     <tabColor indexed="10"/>
   </sheetPr>
-  <dimension ref="A1:S100"/>
+  <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -948,7 +970,7 @@
       </c>
       <c r="S2" s="10"/>
     </row>
-    <row r="3" spans="1:19" ht="78" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="84" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
@@ -3247,10 +3269,10 @@
         <v>64.8</v>
       </c>
       <c r="O98">
-        <v>3.52</v>
+        <v>3.51</v>
       </c>
       <c r="P98">
-        <v>14.7</v>
+        <v>14.9</v>
       </c>
       <c r="R98">
         <v>2.99</v>
@@ -3282,29 +3304,123 @@
         <v>4.16</v>
       </c>
       <c r="K99">
-        <v>10.98</v>
+        <v>10.91</v>
       </c>
       <c r="L99">
         <v>95.9</v>
       </c>
       <c r="M99">
-        <v>7.89</v>
+        <v>7.88</v>
       </c>
       <c r="N99">
         <v>65.400000000000006</v>
       </c>
       <c r="O99">
-        <v>4.1399999999999997</v>
+        <v>4.08</v>
       </c>
       <c r="P99">
-        <v>14.5</v>
+        <v>14.8</v>
       </c>
       <c r="R99">
-        <v>3.52</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14">
+        <v>43281</v>
+      </c>
+      <c r="C100">
+        <v>2.69</v>
+      </c>
+      <c r="D100">
+        <v>2.58</v>
+      </c>
+      <c r="E100">
+        <v>6.56</v>
+      </c>
+      <c r="F100">
+        <v>3.89</v>
+      </c>
+      <c r="G100">
+        <v>3.33</v>
+      </c>
+      <c r="H100">
+        <v>5.2</v>
+      </c>
+      <c r="J100">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="K100">
+        <v>10.5</v>
+      </c>
+      <c r="L100">
+        <v>96</v>
+      </c>
+      <c r="M100">
+        <v>7.78</v>
+      </c>
+      <c r="N100">
+        <v>65.8</v>
+      </c>
+      <c r="O100">
+        <v>4.21</v>
+      </c>
+      <c r="P100">
+        <v>14.3</v>
+      </c>
+      <c r="R100">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A101" s="14">
+        <v>43646</v>
+      </c>
+      <c r="C101">
+        <v>2.54</v>
+      </c>
+      <c r="D101">
+        <v>2.44</v>
+      </c>
+      <c r="E101">
+        <v>7.43</v>
+      </c>
+      <c r="F101">
+        <v>3.64</v>
+      </c>
+      <c r="G101">
+        <v>2.64</v>
+      </c>
+      <c r="H101">
+        <v>5.2</v>
+      </c>
+      <c r="J101">
+        <v>3.8</v>
+      </c>
+      <c r="K101">
+        <v>10.6</v>
+      </c>
+      <c r="L101">
+        <v>96.2</v>
+      </c>
+      <c r="M101">
+        <v>7.64</v>
+      </c>
+      <c r="N101">
+        <v>65.7</v>
+      </c>
+      <c r="O101">
+        <v>3.91</v>
+      </c>
+      <c r="P101">
+        <v>12.8</v>
+      </c>
+      <c r="R101">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A102" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>